<commit_message>
Added Fields for Society Management Page
</commit_message>
<xml_diff>
--- a/MyPremise Fields.xlsx
+++ b/MyPremise Fields.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Society Id</t>
   </si>
@@ -70,13 +71,26 @@
   </si>
   <si>
     <t>Indv. View</t>
+  </si>
+  <si>
+    <t>Members of the society (Multiple/Table) :
+   Name
+   Flat No.
+   Type
+   Contact no</t>
+  </si>
+  <si>
+    <t>Details of fields</t>
+  </si>
+  <si>
+    <t>Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +98,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +123,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -140,12 +168,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -434,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -451,23 +509,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -588,31 +650,18 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
+    <row r="15" spans="1:6" ht="90">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>